<commit_message>
agregados pendientes de la semana
</commit_message>
<xml_diff>
--- a/plan-de-estudio.xlsx
+++ b/plan-de-estudio.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="83">
   <si>
     <t>Lunes</t>
   </si>
@@ -278,6 +278,27 @@
   </si>
   <si>
     <t>historico campeonatos</t>
+  </si>
+  <si>
+    <t>Entrepreneur</t>
+  </si>
+  <si>
+    <t>Viernes 29 de mayo</t>
+  </si>
+  <si>
+    <t>quien es Elon Musk</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Lunes 1 de junio</t>
+  </si>
+  <si>
+    <t>toDoapp</t>
+  </si>
+  <si>
+    <t>weatherApp</t>
   </si>
 </sst>
 </file>
@@ -892,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1034,7 @@
         <v>74</v>
       </c>
       <c r="L3" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>75</v>
@@ -1051,12 +1072,24 @@
         <v>50</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="11"/>
+      <c r="J4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="10">
+        <v>4</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" s="10">
+        <v>1</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -1084,12 +1117,24 @@
         <v>50</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="11"/>
+      <c r="J5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" s="10">
+        <v>7</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" s="10">
+        <v>4</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
@@ -1117,12 +1162,24 @@
         <v>50</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="11"/>
+      <c r="J6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="10">
+        <v>7</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="N6" s="10">
+        <v>5</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">

</xml_diff>

<commit_message>
agrego fechas de proyecto final BD
</commit_message>
<xml_diff>
--- a/plan-de-estudio.xlsx
+++ b/plan-de-estudio.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="89">
   <si>
     <t>Lunes</t>
   </si>
@@ -299,6 +299,24 @@
   </si>
   <si>
     <t>weatherApp</t>
+  </si>
+  <si>
+    <t>Viernes 5 de junio</t>
+  </si>
+  <si>
+    <t>Viernes 10 de julio</t>
+  </si>
+  <si>
+    <t>viernes 7 de agosto</t>
+  </si>
+  <si>
+    <t>Primer entrega PROYECTO FINAL</t>
+  </si>
+  <si>
+    <t>Segunda entrega PROYECTO FINAL</t>
+  </si>
+  <si>
+    <t>Tercer entrega PROYECTO FINAL</t>
   </si>
 </sst>
 </file>
@@ -914,7 +932,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +949,7 @@
     <col min="10" max="10" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" style="1"/>
   </cols>
@@ -1034,7 +1052,7 @@
         <v>74</v>
       </c>
       <c r="L3" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>75</v>
@@ -1079,7 +1097,7 @@
         <v>77</v>
       </c>
       <c r="L4" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>78</v>
@@ -1124,7 +1142,7 @@
         <v>80</v>
       </c>
       <c r="L5" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>81</v>
@@ -1169,7 +1187,7 @@
         <v>80</v>
       </c>
       <c r="L6" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>82</v>
@@ -1207,12 +1225,24 @@
         <v>50</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="11"/>
+      <c r="J7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="10">
+        <v>10</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7" s="10">
+        <v>5</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
@@ -1240,12 +1270,22 @@
         <v>50</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="8"/>
+      <c r="J8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="L8" s="10"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="11"/>
+      <c r="M8" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="N8" s="10">
+        <v>5</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
@@ -1273,12 +1313,22 @@
         <v>27</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="8"/>
+      <c r="J9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="L9" s="10"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="11"/>
+      <c r="M9" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" s="10">
+        <v>5</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">

</xml_diff>

<commit_message>
actualizacion plan semana 1-6 junio
</commit_message>
<xml_diff>
--- a/plan-de-estudio.xlsx
+++ b/plan-de-estudio.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="96">
   <si>
     <t>Lunes</t>
   </si>
@@ -292,15 +292,6 @@
     <t>weatherApp</t>
   </si>
   <si>
-    <t>Viernes 5 de junio</t>
-  </si>
-  <si>
-    <t>Viernes 10 de julio</t>
-  </si>
-  <si>
-    <t>viernes 7 de agosto</t>
-  </si>
-  <si>
     <t>Primer entrega PROYECTO FINAL</t>
   </si>
   <si>
@@ -310,12 +301,6 @@
     <t>Tercer entrega PROYECTO FINAL</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>miercoles 3 de mayo</t>
-  </si>
-  <si>
     <t>DB de supermercado</t>
   </si>
   <si>
@@ -328,7 +313,31 @@
     <t>Sam Walton</t>
   </si>
   <si>
-    <t>Progreso,,,</t>
+    <t>Entregado</t>
+  </si>
+  <si>
+    <t>Progreso…</t>
+  </si>
+  <si>
+    <t>Viernes 12 de junio</t>
+  </si>
+  <si>
+    <t>Viernes 17 de julio</t>
+  </si>
+  <si>
+    <t>viernes 14 de agosto</t>
+  </si>
+  <si>
+    <t>1 mes</t>
+  </si>
+  <si>
+    <t>2 meses</t>
+  </si>
+  <si>
+    <t>miercoles 3 de junio</t>
+  </si>
+  <si>
+    <t>Terminado</t>
   </si>
 </sst>
 </file>
@@ -425,7 +434,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,6 +525,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -559,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -640,14 +655,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +988,7 @@
     <col min="7" max="7" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="40" style="3" bestFit="1" customWidth="1"/>
@@ -976,24 +997,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="J1" s="29" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="J1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -1072,8 +1093,8 @@
       <c r="K3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="10">
-        <v>0</v>
+      <c r="L3" s="32">
+        <v>-6</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>75</v>
@@ -1081,8 +1102,8 @@
       <c r="N3" s="10">
         <v>4</v>
       </c>
-      <c r="O3" s="30" t="s">
-        <v>92</v>
+      <c r="O3" s="28" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1115,19 +1136,19 @@
         <v>40</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="L4" s="10">
         <v>0</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="N4" s="10">
         <v>5</v>
       </c>
-      <c r="O4" s="30" t="s">
-        <v>92</v>
+      <c r="O4" s="31" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1162,8 +1183,8 @@
       <c r="K5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L5" s="10">
-        <v>0</v>
+      <c r="L5" s="32">
+        <v>-3</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>78</v>
@@ -1171,8 +1192,8 @@
       <c r="N5" s="10">
         <v>4</v>
       </c>
-      <c r="O5" s="30" t="s">
-        <v>92</v>
+      <c r="O5" s="28" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1207,8 +1228,8 @@
       <c r="K6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L6" s="10">
-        <v>0</v>
+      <c r="L6" s="32">
+        <v>-3</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>79</v>
@@ -1216,8 +1237,8 @@
       <c r="N6" s="10">
         <v>4</v>
       </c>
-      <c r="O6" s="30" t="s">
-        <v>92</v>
+      <c r="O6" s="28" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1250,19 +1271,19 @@
         <v>40</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="L7" s="10">
         <v>10</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N7" s="10">
         <v>5</v>
       </c>
-      <c r="O7" s="30" t="s">
-        <v>92</v>
+      <c r="O7" s="28" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1295,13 +1316,13 @@
         <v>40</v>
       </c>
       <c r="K8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="N8" s="10">
         <v>5</v>
@@ -1340,13 +1361,13 @@
         <v>40</v>
       </c>
       <c r="K9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="N9" s="10">
         <v>5</v>
@@ -1382,22 +1403,22 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="L10" s="10">
         <v>3</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="N10" s="10">
         <v>1</v>
       </c>
-      <c r="O10" s="12" t="s">
-        <v>42</v>
+      <c r="O10" s="31" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
cambio de plan 4-6-2015
</commit_message>
<xml_diff>
--- a/plan-de-estudio.xlsx
+++ b/plan-de-estudio.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="97">
   <si>
     <t>Lunes</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Terminado</t>
+  </si>
+  <si>
+    <t>Mapa de empatia</t>
   </si>
 </sst>
 </file>
@@ -658,16 +661,16 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -974,7 +977,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,24 +1000,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="J1" s="30" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="J1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -1093,14 +1096,14 @@
       <c r="K3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="32">
+      <c r="L3" s="30">
         <v>-6</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>75</v>
       </c>
       <c r="N3" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O3" s="28" t="s">
         <v>88</v>
@@ -1147,7 +1150,7 @@
       <c r="N4" s="10">
         <v>5</v>
       </c>
-      <c r="O4" s="31" t="s">
+      <c r="O4" s="29" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1183,14 +1186,14 @@
       <c r="K5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="30">
         <v>-3</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>78</v>
       </c>
       <c r="N5" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>88</v>
@@ -1228,14 +1231,14 @@
       <c r="K6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L6" s="32">
+      <c r="L6" s="30">
         <v>-3</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>79</v>
       </c>
       <c r="N6" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O6" s="28" t="s">
         <v>88</v>
@@ -1280,7 +1283,7 @@
         <v>80</v>
       </c>
       <c r="N7" s="10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O7" s="28" t="s">
         <v>88</v>
@@ -1325,7 +1328,7 @@
         <v>81</v>
       </c>
       <c r="N8" s="10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O8" s="12" t="s">
         <v>42</v>
@@ -1370,7 +1373,7 @@
         <v>82</v>
       </c>
       <c r="N9" s="10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O9" s="12" t="s">
         <v>42</v>
@@ -1409,7 +1412,7 @@
         <v>85</v>
       </c>
       <c r="L10" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>86</v>
@@ -1417,7 +1420,7 @@
       <c r="N10" s="10">
         <v>1</v>
       </c>
-      <c r="O10" s="31" t="s">
+      <c r="O10" s="29" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1447,12 +1450,24 @@
         <v>27</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="11"/>
+      <c r="J11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="10">
+        <v>3</v>
+      </c>
+      <c r="O11" s="29" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">

</xml_diff>

<commit_message>
cambio semana 7-13 junio
</commit_message>
<xml_diff>
--- a/plan-de-estudio.xlsx
+++ b/plan-de-estudio.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="92">
   <si>
     <t>Lunes</t>
   </si>
@@ -301,21 +301,6 @@
     <t>Tercer entrega PROYECTO FINAL</t>
   </si>
   <si>
-    <t>DB de supermercado</t>
-  </si>
-  <si>
-    <t>Emprendedurismo</t>
-  </si>
-  <si>
-    <t>viernes 5 de agosto</t>
-  </si>
-  <si>
-    <t>Sam Walton</t>
-  </si>
-  <si>
-    <t>Entregado</t>
-  </si>
-  <si>
     <t>Progreso…</t>
   </si>
   <si>
@@ -334,13 +319,13 @@
     <t>2 meses</t>
   </si>
   <si>
-    <t>miercoles 3 de junio</t>
-  </si>
-  <si>
     <t>Terminado</t>
   </si>
   <si>
-    <t>Mapa de empatia</t>
+    <t>Fundamentos de programacion</t>
+  </si>
+  <si>
+    <t>Ejercicios de algoritmos</t>
   </si>
 </sst>
 </file>
@@ -577,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -672,6 +657,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -976,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +982,7 @@
     <col min="7" max="7" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="40" style="3" bestFit="1" customWidth="1"/>
@@ -1106,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="28" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1136,22 +1127,22 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="4" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="L4" s="30">
+        <v>-3</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="N4" s="10">
         <v>5</v>
       </c>
-      <c r="O4" s="29" t="s">
-        <v>87</v>
+      <c r="O4" s="28" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1190,13 +1181,13 @@
         <v>-3</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N5" s="10">
         <v>5</v>
       </c>
       <c r="O5" s="28" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1226,22 +1217,22 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="4" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="L6" s="30">
-        <v>-3</v>
+        <v>84</v>
+      </c>
+      <c r="L6" s="10">
+        <v>3</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N6" s="10">
-        <v>5</v>
-      </c>
-      <c r="O6" s="28" t="s">
-        <v>88</v>
+        <v>10</v>
+      </c>
+      <c r="O6" s="29" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1274,19 +1265,19 @@
         <v>40</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="L7" s="10">
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N7" s="10">
         <v>10</v>
       </c>
-      <c r="O7" s="28" t="s">
-        <v>88</v>
+      <c r="O7" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1319,13 +1310,13 @@
         <v>40</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N8" s="10">
         <v>10</v>
@@ -1334,7 +1325,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>49</v>
       </c>
@@ -1360,22 +1351,22 @@
         <v>27</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="4" t="s">
-        <v>40</v>
+      <c r="J9" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="K9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="10">
+        <v>3</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="L9" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="N9" s="10">
-        <v>10</v>
-      </c>
-      <c r="O9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="34" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1405,24 +1396,12 @@
         <v>27</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="L10" s="10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="N10" s="10">
-        <v>1</v>
-      </c>
-      <c r="O10" s="29" t="s">
-        <v>95</v>
-      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="11"/>
     </row>
     <row r="11" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
@@ -1450,24 +1429,12 @@
         <v>27</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="L11" s="10">
-        <v>0</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="N11" s="10">
-        <v>3</v>
-      </c>
-      <c r="O11" s="29" t="s">
-        <v>95</v>
-      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">

</xml_diff>

<commit_message>
plan actualizado al 1-10-2015
</commit_message>
<xml_diff>
--- a/plan-de-estudio.xlsx
+++ b/plan-de-estudio.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="79">
   <si>
     <t>Administrador de tiempo</t>
   </si>
@@ -78,21 +78,9 @@
     <t>Bases de datos</t>
   </si>
   <si>
-    <t>1 mes</t>
-  </si>
-  <si>
     <t>3:00am</t>
   </si>
   <si>
-    <t>viernes 14 de agosto</t>
-  </si>
-  <si>
-    <t>tercer entrega PROYECTO FINAL</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
     <t>4:00am</t>
   </si>
   <si>
@@ -249,58 +237,22 @@
     <t>Lenguje Servidor - PHP</t>
   </si>
   <si>
-    <t>PHP</t>
-  </si>
-  <si>
-    <t>viernes 24 de julio</t>
-  </si>
-  <si>
-    <t>2 semanas</t>
-  </si>
-  <si>
-    <t>inventario</t>
-  </si>
-  <si>
-    <t>En progreso</t>
-  </si>
-  <si>
-    <t>Side Project</t>
-  </si>
-  <si>
-    <t>10 días</t>
-  </si>
-  <si>
-    <t>Descubrir como integrar juegos en una pagina web</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Revisar Portafolio</t>
-  </si>
-  <si>
-    <t>Revisar y hacer cambios necesarios al portafolio para que sea totalmente funcional</t>
-  </si>
-  <si>
-    <t>Viernes 31 julio</t>
-  </si>
-  <si>
-    <t>Realizar prototipo funcional del app  para onebook</t>
-  </si>
-  <si>
-    <t>Emprendedurismo</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisar documentacion relacionada con AJAX </t>
-  </si>
-  <si>
-    <t>Terminar los selects de la base de datos</t>
-  </si>
-  <si>
-    <t>Hacer tarea, instrucciones en moodle</t>
+    <t>RWD</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>Revisar la asignacion de nuevas tareas</t>
+  </si>
+  <si>
+    <t>Terminar el blog</t>
+  </si>
+  <si>
+    <t>instalar vagrant y drupal en windows 10</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -394,7 +346,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,18 +381,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
         <bgColor rgb="FFB3A2C7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF009933"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF558ED5"/>
-        <bgColor rgb="FF45818E"/>
       </patternFill>
     </fill>
     <fill>
@@ -534,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -569,19 +509,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -590,48 +524,48 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1004,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,14 +963,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -1078,22 +1012,18 @@
     </row>
     <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="11">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="12">
-        <v>6</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -1107,22 +1037,18 @@
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="12">
-        <v>10</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>24</v>
+        <v>73</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="11">
+        <v>8</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
@@ -1134,24 +1060,20 @@
       <c r="N4"/>
       <c r="O4"/>
     </row>
-    <row r="5" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="12">
+        <v>74</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="11">
         <v>10</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>24</v>
+      <c r="F5" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -1163,25 +1085,13 @@
       <c r="N5"/>
       <c r="O5"/>
     </row>
-    <row r="6" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="11">
-        <v>5</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>24</v>
-      </c>
+    <row r="6" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
@@ -1192,25 +1102,13 @@
       <c r="N6"/>
       <c r="O6"/>
     </row>
-    <row r="7" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="11">
-        <v>3</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="11">
-        <v>5</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>24</v>
-      </c>
+    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -1221,23 +1119,13 @@
       <c r="N7"/>
       <c r="O7"/>
     </row>
-    <row r="8" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>92</v>
-      </c>
+    <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="14" t="s">
-        <v>24</v>
-      </c>
+      <c r="F8" s="12"/>
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
@@ -1249,24 +1137,12 @@
       <c r="O8"/>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="11">
-        <v>3</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="12">
-        <v>6</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>81</v>
-      </c>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -1278,24 +1154,12 @@
       <c r="O9"/>
     </row>
     <row r="10" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="11">
-        <v>3</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="12">
-        <v>10</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>24</v>
-      </c>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
@@ -1310,9 +1174,9 @@
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="18"/>
+      <c r="F11" s="16"/>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
@@ -1327,9 +1191,9 @@
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
-      <c r="D12" s="15"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="18"/>
+      <c r="F12" s="16"/>
       <c r="G12"/>
       <c r="H12"/>
       <c r="I12"/>
@@ -1344,9 +1208,9 @@
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="18"/>
+      <c r="F13" s="16"/>
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13"/>
@@ -1361,9 +1225,9 @@
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="18"/>
+      <c r="F14" s="16"/>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
@@ -1378,9 +1242,9 @@
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="15"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="18"/>
+      <c r="F15" s="16"/>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
@@ -1395,9 +1259,9 @@
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="18"/>
+      <c r="F16" s="16"/>
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
@@ -1412,9 +1276,9 @@
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="18"/>
+      <c r="F17" s="16"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
@@ -1429,9 +1293,9 @@
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="18"/>
+      <c r="F18" s="16"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
@@ -1446,9 +1310,9 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="15"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="18"/>
+      <c r="F19" s="16"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
@@ -1583,335 +1447,335 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.7109375" style="21"/>
-    <col min="2" max="2" width="30" style="21"/>
-    <col min="3" max="3" width="28.7109375" style="21"/>
+    <col min="1" max="1" width="63.7109375" style="19"/>
+    <col min="2" max="2" width="30" style="19"/>
+    <col min="3" max="3" width="28.7109375" style="19"/>
     <col min="4" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C2" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="23" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="B4" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B5" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="24">
+        <v>0</v>
+      </c>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="B6" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="B7" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B8" s="24">
         <v>0.2</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C8" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26">
+        <v>1</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="26">
+      <c r="B12" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C14" s="24">
         <v>0</v>
       </c>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C16" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C18" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C19" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="26">
+        <v>1</v>
+      </c>
+      <c r="C20" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+    </row>
+    <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="C6" s="26">
+      <c r="C23" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C25" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="C7" s="26">
+    <row r="26" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C26" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="C8" s="26">
+    <row r="27" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C27" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28">
+    <row r="28" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C28" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C29" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C30" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="26">
         <v>1</v>
       </c>
-      <c r="C9" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-    </row>
-    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="C14" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="C15" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="C16" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="C17" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="C18" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="C19" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="28">
-        <v>1</v>
-      </c>
-      <c r="C20" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-    </row>
-    <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="C25" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="C26" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="C27" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="C28" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="C29" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="C30" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28">
-        <v>1</v>
-      </c>
-      <c r="C31" s="28">
+      <c r="C31" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2023,7 +1887,7 @@
     </row>
     <row r="5" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>17</v>
@@ -2049,7 +1913,7 @@
     </row>
     <row r="6" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>17</v>
@@ -2075,7 +1939,7 @@
     </row>
     <row r="7" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>17</v>
@@ -2101,22 +1965,22 @@
     </row>
     <row r="8" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>17</v>
@@ -2127,423 +1991,423 @@
     </row>
     <row r="9" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>28</v>
+      <c r="B11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>45</v>
+      <c r="B19" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>28</v>
+        <v>45</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>31</v>
+        <v>47</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>17</v>
@@ -2560,16 +2424,16 @@
       <c r="F25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>28</v>
+      <c r="G25" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>17</v>

</xml_diff>